<commit_message>
replace sd card slot
</commit_message>
<xml_diff>
--- a/hardware/rev_c/embedded-gw_bom.xlsx
+++ b/hardware/rev_c/embedded-gw_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="152">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -46,12 +46,12 @@
     <t xml:space="preserve">MANUFACTURER</t>
   </si>
   <si>
+    <t xml:space="preserve">MOUSER</t>
+  </si>
+  <si>
     <t xml:space="preserve">MPN</t>
   </si>
   <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
     <t xml:space="preserve">DIODE_ZENER0201</t>
   </si>
   <si>
@@ -223,6 +223,18 @@
     <t xml:space="preserve">RC0402FR-07470RL</t>
   </si>
   <si>
+    <t xml:space="preserve">J1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONN MICRO SD CARD PUSH-PUSH R/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WM24066CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molex</t>
+  </si>
+  <si>
     <t xml:space="preserve">ABS05-32.768KHZ-9-T</t>
   </si>
   <si>
@@ -328,31 +340,13 @@
     <t xml:space="preserve">A cheap, simple USB to UART adapter</t>
   </si>
   <si>
-    <t xml:space="preserve">336-3692-ND</t>
+    <t xml:space="preserve">336-5885-ND</t>
   </si>
   <si>
     <t xml:space="preserve">SiLabs</t>
   </si>
   <si>
-    <t xml:space="preserve">CP2102N-A01-GQFN20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DM3BT-DSF-PEJS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HRS_DM3BT-DSF-PEJS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 (8 + 2) Position Card Connector Secure Digital - microSD™ Surface Mount, Right Angle Gold Check prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR1942TR-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hirose Connector</t>
+    <t xml:space="preserve">CP2102N-A02-GQFN20</t>
   </si>
   <si>
     <t xml:space="preserve">EMIF06-MSD01F2</t>
@@ -373,6 +367,9 @@
     <t xml:space="preserve">STMicroelectronics</t>
   </si>
   <si>
+    <t xml:space="preserve">511-EMIF06-MSD01F2</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESDR0502N</t>
   </si>
   <si>
@@ -430,6 +427,12 @@
     <t xml:space="preserve">2.5V Drive Nch+Nch MOSFET</t>
   </si>
   <si>
+    <t xml:space="preserve">QS5K2CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohm</t>
+  </si>
+  <si>
     <t xml:space="preserve">RED</t>
   </si>
   <si>
@@ -440,18 +443,6 @@
   </si>
   <si>
     <t xml:space="preserve">LTST-C193KRKT-5A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC2030-JLINK-NL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC2030-IDC-NL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNI</t>
   </si>
   <si>
     <t xml:space="preserve">USB-A-MALE-PLUG</t>
@@ -580,10 +571,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -592,10 +583,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="20.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="30.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="98.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="98.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,7 +638,7 @@
       <c r="G2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -672,7 +664,7 @@
       <c r="G3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>21</v>
       </c>
     </row>
@@ -698,7 +690,7 @@
       <c r="G4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>25</v>
       </c>
     </row>
@@ -724,7 +716,7 @@
       <c r="G5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="J5" s="0" t="s">
         <v>31</v>
       </c>
     </row>
@@ -750,7 +742,7 @@
       <c r="G6" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="J6" s="0" t="s">
         <v>35</v>
       </c>
     </row>
@@ -776,7 +768,7 @@
       <c r="G7" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="J7" s="0" t="s">
         <v>41</v>
       </c>
     </row>
@@ -802,7 +794,7 @@
       <c r="G8" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="J8" s="0" t="s">
         <v>45</v>
       </c>
     </row>
@@ -828,7 +820,7 @@
       <c r="G9" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="J9" s="0" t="s">
         <v>49</v>
       </c>
     </row>
@@ -854,7 +846,7 @@
       <c r="G10" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="J10" s="0" t="s">
         <v>53</v>
       </c>
     </row>
@@ -880,7 +872,7 @@
       <c r="G11" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="J11" s="0" t="s">
         <v>59</v>
       </c>
     </row>
@@ -906,7 +898,7 @@
       <c r="G12" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="J12" s="0" t="s">
         <v>63</v>
       </c>
     </row>
@@ -932,7 +924,7 @@
       <c r="G13" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="J13" s="0" t="s">
         <v>66</v>
       </c>
     </row>
@@ -940,29 +932,29 @@
       <c r="A14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="0" t="n">
+        <v>5027740891</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>5027740891</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>5027740891</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="0" t="s">
+      <c r="F14" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>67</v>
+      <c r="J14" s="0" t="n">
+        <v>5027740891</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -970,112 +962,112 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="G15" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="H15" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>79</v>
+      <c r="J15" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="G16" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="H16" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="J16" s="0" t="s">
         <v>83</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="G17" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="H17" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>91</v>
+      <c r="J17" s="0" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="0" t="s">
+      <c r="F18" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="G18" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="J18" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,28 +1075,28 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="D19" s="0" t="s">
+      <c r="F19" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="G19" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="H19" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="G19" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>104</v>
+      <c r="J19" s="0" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1112,28 +1104,28 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20" s="0" t="s">
+      <c r="G20" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="H20" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="J20" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="H20" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="I20" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1141,28 +1133,31 @@
         <v>1</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="F21" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="G21" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="H21" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="I21" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>111</v>
+      <c r="J21" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,22 +1165,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="0" t="s">
+      <c r="E22" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="G22" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="J22" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,25 +1188,25 @@
         <v>2</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="G23" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="H23" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="J23" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,28 +1214,28 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="0" t="s">
+      <c r="F24" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="F24" s="0" t="s">
+      <c r="G24" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="H24" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="H24" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>127</v>
+      <c r="J24" s="0" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1248,19 +1243,28 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="D25" s="0" t="s">
+      <c r="E25" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="F25" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="F25" s="0" t="s">
+      <c r="G25" s="0" t="s">
         <v>135</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1268,25 +1272,25 @@
         <v>3</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="I26" s="0" t="s">
         <v>139</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,74 +1298,54 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>146</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>147</v>
+        <v>93</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="I28" s="0" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B29" s="0" t="s">
+      <c r="J28" s="0" t="s">
         <v>151</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>